<commit_message>
done v1 (main_v0.py, main_v1.py)
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/example/example_input.xlsx
+++ b/6_TuningWith2Prompting/example/example_input.xlsx
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +101,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -152,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -169,14 +175,14 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -196,29 +202,32 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,7 +538,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="50.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="23" width="50.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="9" width="72.57642857142856" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -586,42 +595,42 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="45.75" customFormat="1" s="19">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="19">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>

</xml_diff>